<commit_message>
Added original format (hardcoded)
</commit_message>
<xml_diff>
--- a/output/movies.xlsx
+++ b/output/movies.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="105">
   <si>
     <t>TitleCode</t>
   </si>
@@ -95,6 +95,9 @@
     <t>ShortSynopsis</t>
   </si>
   <si>
+    <t>OriginalFormat</t>
+  </si>
+  <si>
     <t>tt0086879</t>
   </si>
   <si>
@@ -117,6 +120,9 @@
   </si>
   <si>
     <t>The incredible story of genius musician Wolfgang Amadeus Mozart, told in flashback by his peer and secret rival Antonio Salieri – now confined to an insane asylum.</t>
+  </si>
+  <si>
+    <t>35mm</t>
   </si>
   <si>
     <t>F. Murray Abraham</t>
@@ -688,26 +694,26 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -741,13 +747,13 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -781,123 +787,123 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
         <v>35</v>
-      </c>
-      <c r="C4" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -927,10 +933,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -960,26 +966,26 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1009,10 +1015,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1050,282 +1056,282 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D6" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C9" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D9" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C10" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D10" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C12" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D12" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D13" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C16" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D16" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D17" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D18" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D19" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C20" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D20" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C21" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D21" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1335,7 +1341,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1355,9 +1361,10 @@
     <col min="12" max="12" width="30.7109375" customWidth="1"/>
     <col min="13" max="13" width="10.7109375" customWidth="1"/>
     <col min="14" max="14" width="100.7109375" customWidth="1"/>
+    <col min="15" max="15" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1400,46 +1407,52 @@
       <c r="N1" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="O1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G2">
         <v>18000000</v>
       </c>
       <c r="H2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I2">
         <v>51973029</v>
       </c>
       <c r="J2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K2">
         <v>160</v>
       </c>
       <c r="M2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N2" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="O2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>